<commit_message>
pandas processing for database tables
</commit_message>
<xml_diff>
--- a/Database structure.xlsx
+++ b/Database structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="ERD" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="556">
   <si>
     <t>Field</t>
   </si>
@@ -1303,9 +1303,6 @@
     <t>details (for mcd/env)</t>
   </si>
   <si>
-    <t>This is essentially an EAV format</t>
-  </si>
-  <si>
     <t>which I think makes sense because most of these attributes are sparse</t>
   </si>
   <si>
@@ -1402,9 +1399,6 @@
     <t>&lt;10% of all PRJ records, and 2% of all records.  More typically about 0.2%</t>
   </si>
   <si>
-    <t>PRJ records only</t>
-  </si>
-  <si>
     <t>quarter*</t>
   </si>
   <si>
@@ -1640,13 +1634,76 @@
   </si>
   <si>
     <t>related_building_permit</t>
+  </si>
+  <si>
+    <t>mcd/env details</t>
+  </si>
+  <si>
+    <t>Key for project descriptions. This table contains the subset of project descriptions which contain additional details</t>
+  </si>
+  <si>
+    <t>MCD_REFERRAL and ENVIRONMENTAL_REVIEW_TYPE have categoricals instead of just "checked or unchecked".</t>
+  </si>
+  <si>
+    <t>ADU area</t>
+  </si>
+  <si>
+    <t>key for dwelling unit changes</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>0-1 to 1-m</t>
+  </si>
+  <si>
+    <t>1 to 1-m</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>1 to 0-1</t>
+  </si>
+  <si>
+    <t>0-m</t>
+  </si>
+  <si>
+    <t>1 to</t>
+  </si>
+  <si>
+    <t>The right side is in EAV format</t>
+  </si>
+  <si>
+    <t>rename feature to include this field</t>
+  </si>
+  <si>
+    <t>land_use</t>
+  </si>
+  <si>
+    <t>prj_feature</t>
+  </si>
+  <si>
+    <t>dwelling</t>
+  </si>
+  <si>
+    <t>prj_desc</t>
+  </si>
+  <si>
+    <t>PRJ_FEATURE_STORIES_EXIST</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>prj_desc_detail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1669,6 +1726,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1684,7 +1757,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1741,51 +1814,6 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1862,59 +1890,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1958,1079 +2058,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1933575" y="657225"/>
-          <a:ext cx="542925" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1943100" y="876300"/>
-          <a:ext cx="552450" cy="1333501"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1857375" y="552450"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="256160" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1857375" y="1828800"/>
-          <a:ext cx="256160" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="256160" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1838325" y="1819275"/>
-          <a:ext cx="256160" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="256160" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="TextBox 12"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4867275" y="3152775"/>
-          <a:ext cx="256160" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="TextBox 14"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2143125" y="1076325"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1724025</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="TextBox 15"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4238625" y="857250"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="TextBox 31"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7419975" y="533400"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1781175</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="256160" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="TextBox 32"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4295775" y="466725"/>
-          <a:ext cx="256160" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="TextBox 44"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7429500" y="2009775"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="TextBox 45"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7458075" y="3686175"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="47" name="Straight Arrow Connector 46"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1914525" y="1257300"/>
-          <a:ext cx="581025" cy="2495551"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="256160" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="TextBox 52"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2324100" y="390525"/>
-          <a:ext cx="256160" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1781175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Elbow Connector 6"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4295775" y="685800"/>
-          <a:ext cx="3524250" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 85135"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1781175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Elbow Connector 25"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4295775" y="695325"/>
-          <a:ext cx="3495675" cy="1762125"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 85967"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1781175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Elbow Connector 28"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4295775" y="695325"/>
-          <a:ext cx="3505200" cy="3286125"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 85598"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1768793</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>773240</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>74105</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="35" name="Elbow Connector 34"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4283393" y="690563"/>
-          <a:ext cx="804672" cy="1536192"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 66572"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1768793</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>773240</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>56960</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="43" name="Elbow Connector 42"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4283393" y="690563"/>
-          <a:ext cx="804672" cy="1719072"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 65388"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="412036" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="TextBox 43"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4752975" y="2000250"/>
-          <a:ext cx="412036" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0-m</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6668</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>11240</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>88583</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="Elbow Connector 47"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4321493" y="1071563"/>
-          <a:ext cx="804672" cy="2331720"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 25142"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3296,350 +2323,642 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J29"/>
+  <dimension ref="B1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="37" t="s">
+        <v>513</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C4" s="27"/>
+      <c r="D4" s="37" t="s">
+        <v>337</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="35" t="s">
+        <v>507</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="37" t="s">
+        <v>376</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="35" t="s">
+        <v>382</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>546</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>545</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>508</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>542</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="41" t="s">
+        <v>545</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>509</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+    </row>
+    <row r="7" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="36" t="s">
+        <v>543</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="35" t="s">
+        <v>405</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="43" t="s">
+        <v>545</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="27"/>
+      <c r="D11" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="36" t="s">
+        <v>518</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>542</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="36" t="s">
+        <v>519</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="36" t="s">
+        <v>394</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="33" t="s">
+        <v>520</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="37" t="s">
+        <v>550</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="27"/>
+      <c r="D17" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="30" t="s">
+        <v>545</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>541</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="36" t="s">
+        <v>415</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="36" t="s">
+        <v>521</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>456</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="36" t="s">
+        <v>522</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="36" t="s">
+        <v>393</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="26"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="26"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="37" t="s">
+        <v>551</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>544</v>
+      </c>
+      <c r="I25" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="H26" s="27"/>
+      <c r="I26" s="30" t="s">
+        <v>527</v>
+      </c>
+      <c r="J26" s="27"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="36" t="s">
+        <v>413</v>
+      </c>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="36" t="s">
+        <v>524</v>
+      </c>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="28" t="s">
+        <v>417</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="M29" s="27"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="33" t="s">
+        <v>526</v>
+      </c>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="O31" s="26"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F32" s="46"/>
+      <c r="G32" s="34" t="s">
+        <v>552</v>
+      </c>
+      <c r="I32" s="31" t="s">
+        <v>555</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="46"/>
+      <c r="G33" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="F4" t="s">
-        <v>457</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="J4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="H33" s="30" t="s">
+        <v>544</v>
+      </c>
+      <c r="I33" s="29" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F34" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G34" s="32" t="s">
         <v>407</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="J5" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="I34" s="30" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="H9" s="9" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>509</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>510</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>511</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="3" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="8" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>506</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>417</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B29:C29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>381</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>382</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D2" t="s">
         <v>334</v>
       </c>
       <c r="E2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3647,13 +2966,13 @@
         <v>383</v>
       </c>
       <c r="C3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D3" t="s">
         <v>334</v>
       </c>
       <c r="E3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3661,13 +2980,13 @@
         <v>384</v>
       </c>
       <c r="C4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D4" t="s">
         <v>334</v>
       </c>
       <c r="E4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3675,13 +2994,13 @@
         <v>385</v>
       </c>
       <c r="C5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D5" t="s">
         <v>335</v>
       </c>
       <c r="E5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,7 +3011,7 @@
         <v>335</v>
       </c>
       <c r="E6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3703,7 +3022,7 @@
         <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3714,7 +3033,7 @@
         <v>336</v>
       </c>
       <c r="E8" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3725,7 +3044,7 @@
         <v>336</v>
       </c>
       <c r="E9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,7 +3055,7 @@
         <v>335</v>
       </c>
       <c r="E10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3747,7 +3066,7 @@
         <v>335</v>
       </c>
       <c r="E11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3785,13 +3104,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D15" t="s">
         <v>335</v>
       </c>
       <c r="E15" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3802,7 +3121,7 @@
         <v>334</v>
       </c>
       <c r="E16" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3813,7 +3132,7 @@
         <v>334</v>
       </c>
       <c r="E17" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3824,24 +3143,24 @@
         <v>334</v>
       </c>
       <c r="E18" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>386</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>390</v>
       </c>
       <c r="C20" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D20" t="s">
         <v>334</v>
       </c>
       <c r="E20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3852,7 +3171,7 @@
         <v>335</v>
       </c>
       <c r="E21" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3863,7 +3182,7 @@
         <v>335</v>
       </c>
       <c r="E22" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3874,7 +3193,7 @@
         <v>335</v>
       </c>
       <c r="E23" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3885,24 +3204,24 @@
         <v>335</v>
       </c>
       <c r="E24" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>388</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>391</v>
       </c>
       <c r="C26" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D26" t="s">
         <v>335</v>
       </c>
       <c r="E26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,46 +3232,46 @@
         <v>335</v>
       </c>
       <c r="E27" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D28" t="s">
         <v>335</v>
       </c>
       <c r="E28" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D29" t="s">
         <v>335</v>
       </c>
       <c r="E29" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>387</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>389</v>
       </c>
       <c r="C31" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D31" t="s">
         <v>334</v>
       </c>
       <c r="E31" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3963,7 +3282,7 @@
         <v>335</v>
       </c>
       <c r="E32" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3974,46 +3293,46 @@
         <v>335</v>
       </c>
       <c r="E33" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D34" t="s">
         <v>359</v>
       </c>
       <c r="E34" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D35" t="s">
         <v>359</v>
       </c>
       <c r="E35" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>401</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>414</v>
       </c>
       <c r="C37" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D37" t="s">
         <v>334</v>
       </c>
       <c r="E37" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4021,13 +3340,13 @@
         <v>407</v>
       </c>
       <c r="C38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D38" t="s">
         <v>334</v>
       </c>
       <c r="E38" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -4038,35 +3357,35 @@
         <v>335</v>
       </c>
       <c r="E39" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="8" t="s">
         <v>423</v>
       </c>
       <c r="D40" t="s">
         <v>335</v>
       </c>
       <c r="E40" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>404</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>405</v>
       </c>
       <c r="C42" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D42" t="s">
         <v>334</v>
       </c>
       <c r="E42" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -4074,13 +3393,13 @@
         <v>407</v>
       </c>
       <c r="C43" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D43" t="s">
         <v>334</v>
       </c>
       <c r="E43" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -4091,57 +3410,57 @@
         <v>335</v>
       </c>
       <c r="E44" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" t="s">
-        <v>520</v>
+      <c r="B45" s="6" t="s">
+        <v>518</v>
       </c>
       <c r="D45" t="s">
         <v>359</v>
       </c>
       <c r="E45" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
-        <v>521</v>
+      <c r="B46" s="6" t="s">
+        <v>519</v>
       </c>
       <c r="D46" t="s">
         <v>359</v>
       </c>
       <c r="E46" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="s">
-        <v>522</v>
+      <c r="B47" s="7" t="s">
+        <v>520</v>
       </c>
       <c r="D47" t="s">
         <v>359</v>
       </c>
       <c r="E47" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>408</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>409</v>
       </c>
       <c r="C49" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D49" t="s">
         <v>334</v>
       </c>
       <c r="E49" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4149,13 +3468,13 @@
         <v>407</v>
       </c>
       <c r="C50" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D50" t="s">
         <v>334</v>
       </c>
       <c r="E50" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4166,57 +3485,57 @@
         <v>335</v>
       </c>
       <c r="E51" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="8" t="s">
-        <v>523</v>
+      <c r="B52" s="6" t="s">
+        <v>521</v>
       </c>
       <c r="D52" t="s">
         <v>334</v>
       </c>
       <c r="E52" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="8" t="s">
-        <v>524</v>
+      <c r="B53" s="6" t="s">
+        <v>522</v>
       </c>
       <c r="D53" t="s">
         <v>334</v>
       </c>
       <c r="E53" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
-        <v>525</v>
+      <c r="B54" s="7" t="s">
+        <v>523</v>
       </c>
       <c r="D54" t="s">
         <v>334</v>
       </c>
       <c r="E54" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="5" t="s">
         <v>411</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>412</v>
       </c>
       <c r="C56" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D56" t="s">
         <v>334</v>
       </c>
       <c r="E56" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -4224,13 +3543,13 @@
         <v>407</v>
       </c>
       <c r="C57" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D57" t="s">
         <v>334</v>
       </c>
       <c r="E57" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -4241,97 +3560,164 @@
         <v>335</v>
       </c>
       <c r="E58" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D59" t="s">
         <v>334</v>
       </c>
       <c r="E59" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D60" t="s">
         <v>334</v>
       </c>
       <c r="E60" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="8" t="s">
-        <v>528</v>
+      <c r="B61" s="6" t="s">
+        <v>526</v>
       </c>
       <c r="D61" t="s">
         <v>334</v>
       </c>
       <c r="E61" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D62" t="s">
         <v>359</v>
       </c>
       <c r="E62" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>509</v>
+      <c r="A64" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>507</v>
       </c>
       <c r="C64" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D64" t="s">
         <v>334</v>
       </c>
       <c r="E64" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="19" t="s">
-        <v>510</v>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="12" t="s">
+        <v>508</v>
       </c>
       <c r="C65" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D65" t="s">
         <v>334</v>
       </c>
       <c r="E65" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
+        <v>509</v>
       </c>
       <c r="C66" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D66" t="s">
         <v>334</v>
       </c>
       <c r="E66" t="s">
-        <v>513</v>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
+        <v>535</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="23" t="s">
+        <v>538</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="19"/>
+      <c r="B72" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -4344,8 +3730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4361,7 +3747,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4373,10 +3759,10 @@
         <v>362</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>330</v>
@@ -4413,25 +3799,25 @@
         <v>376</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <f>A3+1</f>
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>428</v>
+      <c r="H4" s="9" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4452,10 +3838,10 @@
         <v>337</v>
       </c>
       <c r="G5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4494,7 +3880,7 @@
         <v>337</v>
       </c>
       <c r="G7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4515,7 +3901,7 @@
         <v>337</v>
       </c>
       <c r="G8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4536,7 +3922,7 @@
         <v>376</v>
       </c>
       <c r="G9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4557,7 +3943,7 @@
         <v>342</v>
       </c>
       <c r="G10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4578,24 +3964,24 @@
         <v>342</v>
       </c>
       <c r="G11" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="9" t="s">
         <v>347</v>
       </c>
     </row>
@@ -4635,21 +4021,21 @@
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="9" t="s">
         <v>380</v>
       </c>
     </row>
@@ -4671,7 +4057,7 @@
         <v>337</v>
       </c>
       <c r="H16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4713,98 +4099,98 @@
         <v>338</v>
       </c>
       <c r="H18" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="9" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12">
+    <row r="20" spans="1:8" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
+      <c r="H20" s="9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
         <v>18</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="17" t="s">
         <v>334</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="F21" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="16" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="H22" s="17" t="s">
         <v>516</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
-        <v>19</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>515</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>517</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4825,10 +4211,10 @@
         <v>337</v>
       </c>
       <c r="F23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G23" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4849,7 +4235,7 @@
         <v>338</v>
       </c>
       <c r="G24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4870,7 +4256,7 @@
         <v>338</v>
       </c>
       <c r="G25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4891,7 +4277,7 @@
         <v>338</v>
       </c>
       <c r="G26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4941,13 +4327,13 @@
         <v>337</v>
       </c>
       <c r="F30" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G30" t="s">
         <v>357</v>
       </c>
       <c r="H30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4962,7 +4348,7 @@
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4977,7 +4363,7 @@
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5004,7 +4390,7 @@
         <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -5070,7 +4456,7 @@
         <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -5085,7 +4471,7 @@
         <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -5112,7 +4498,7 @@
         <v>67</v>
       </c>
       <c r="F42" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -5238,7 +4624,7 @@
         <v>340</v>
       </c>
       <c r="F52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H52" t="s">
         <v>356</v>
@@ -5271,7 +4657,7 @@
         <v>340</v>
       </c>
       <c r="F54" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H54" t="s">
         <v>358</v>
@@ -5282,13 +4668,13 @@
         <v>360</v>
       </c>
       <c r="D56" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E56" t="s">
         <v>354</v>
       </c>
       <c r="F56" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G56" t="s">
         <v>366</v>
@@ -5593,7 +4979,7 @@
         <v>354</v>
       </c>
       <c r="F82" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G82" t="s">
         <v>366</v>
@@ -5749,7 +5135,7 @@
         <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>553</v>
       </c>
       <c r="C95" t="s">
         <v>165</v>
@@ -5761,13 +5147,13 @@
         <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C96" t="s">
         <v>167</v>
       </c>
       <c r="G96" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -5776,7 +5162,7 @@
         <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C97" t="s">
         <v>169</v>
@@ -5842,7 +5228,7 @@
         <v>178</v>
       </c>
       <c r="G102" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -6049,10 +5435,10 @@
         <v>211</v>
       </c>
       <c r="F119" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H119" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -6067,7 +5453,7 @@
         <v>213</v>
       </c>
       <c r="F120" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -6082,7 +5468,7 @@
         <v>215</v>
       </c>
       <c r="F121" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -6097,7 +5483,7 @@
         <v>217</v>
       </c>
       <c r="F122" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -6112,7 +5498,7 @@
         <v>219</v>
       </c>
       <c r="F123" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -6127,7 +5513,7 @@
         <v>221</v>
       </c>
       <c r="F124" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -6142,7 +5528,7 @@
         <v>223</v>
       </c>
       <c r="F125" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -6157,7 +5543,7 @@
         <v>225</v>
       </c>
       <c r="F126" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -6172,79 +5558,70 @@
         <v>227</v>
       </c>
       <c r="F127" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="18">
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
-      <c r="B128" s="25" t="s">
+      <c r="B128" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C128" s="25" t="s">
+      <c r="C128" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="D128" s="25" t="s">
+      <c r="D128" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="F128" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="G128" s="25" t="s">
-        <v>347</v>
-      </c>
-      <c r="H128" s="25" t="s">
+      <c r="F128" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="G128" t="s">
+        <v>548</v>
+      </c>
+      <c r="H128" s="18" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="129" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="25">
+    <row r="129" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="18">
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B129" s="25" t="s">
+      <c r="B129" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="C129" s="25" t="s">
+      <c r="C129" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="G129" s="25" t="s">
-        <v>347</v>
-      </c>
-      <c r="H129" s="25" t="s">
+      <c r="H129" s="18" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="25">
+    <row r="130" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="18">
         <f t="shared" si="3"/>
         <v>121</v>
       </c>
-      <c r="B130" s="25" t="s">
+      <c r="B130" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="C130" s="25" t="s">
+      <c r="C130" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="G130" s="25" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="25">
+    </row>
+    <row r="131" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="18">
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="B131" s="25" t="s">
+      <c r="B131" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="C131" s="25" t="s">
+      <c r="C131" s="18" t="s">
         <v>235</v>
-      </c>
-      <c r="G131" s="25" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6258,7 +5635,7 @@
         <v>354</v>
       </c>
       <c r="F133" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G133" t="s">
         <v>366</v>
@@ -6459,7 +5836,7 @@
         <v>359</v>
       </c>
       <c r="H149" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6513,7 +5890,7 @@
         <v>359</v>
       </c>
       <c r="H153" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6567,7 +5944,7 @@
         <v>359</v>
       </c>
       <c r="H157" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6621,7 +5998,7 @@
         <v>359</v>
       </c>
       <c r="H161" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -6744,7 +6121,7 @@
         <v>311</v>
       </c>
       <c r="F171" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -6759,7 +6136,7 @@
         <v>313</v>
       </c>
       <c r="F172" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -6774,7 +6151,7 @@
         <v>315</v>
       </c>
       <c r="F173" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -6800,141 +6177,141 @@
         <v>337</v>
       </c>
       <c r="F176" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G176" t="s">
         <v>368</v>
       </c>
       <c r="H176" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="12">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="9">
         <f t="shared" ref="A177:A184" si="5">A176+1</f>
         <v>164</v>
       </c>
-      <c r="B177" s="12" t="s">
+      <c r="B177" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C177" s="12" t="s">
+      <c r="C177" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="F177" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="G177" s="12" t="s">
+      <c r="F177" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="G177" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="H177" s="12" t="s">
+      <c r="H177" s="9" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="178" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="12">
+    <row r="178" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="9">
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="B178" s="12" t="s">
+      <c r="B178" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C178" s="12" t="s">
+      <c r="C178" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="F178" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="G178" s="12" t="s">
+      <c r="F178" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="G178" s="9" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="12">
+    <row r="179" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="9">
         <f t="shared" si="5"/>
         <v>166</v>
       </c>
-      <c r="B179" s="12" t="s">
+      <c r="B179" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="C179" s="12" t="s">
+      <c r="C179" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="F179" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="G179" s="12" t="s">
+      <c r="F179" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="G179" s="9" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="12">
+    <row r="180" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="9">
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="B180" s="12" t="s">
+      <c r="B180" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="C180" s="12" t="s">
+      <c r="C180" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="D180" s="12" t="s">
+      <c r="D180" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="F180" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="G180" s="12" t="s">
+      <c r="F180" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="H180" s="12" t="s">
+      <c r="G180" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="H180" s="9" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="181" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="12">
+    <row r="181" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="9">
         <f t="shared" si="5"/>
         <v>168</v>
       </c>
-      <c r="B181" s="12" t="s">
+      <c r="B181" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C181" s="12" t="s">
+      <c r="C181" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="D181" s="12" t="s">
+      <c r="D181" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="F181" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="G181" s="12" t="s">
+      <c r="F181" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="H181" s="12" t="s">
+      <c r="G181" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="H181" s="9" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="12">
+    <row r="182" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="9">
         <f t="shared" si="5"/>
         <v>169</v>
       </c>
-      <c r="B182" s="12" t="s">
+      <c r="B182" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="C182" s="12" t="s">
+      <c r="C182" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="D182" s="12" t="s">
+      <c r="D182" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="F182" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="G182" s="12" t="s">
+      <c r="F182" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="H182" s="12" t="s">
+      <c r="G182" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="H182" s="9" t="s">
         <v>372</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish code to generate database
</commit_message>
<xml_diff>
--- a/Database structure.xlsx
+++ b/Database structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="10545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="10545" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ERD" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="545">
   <si>
     <t>Field</t>
   </si>
@@ -1174,9 +1174,6 @@
     <t>remove, because it's redundant</t>
   </si>
   <si>
-    <t>Record</t>
-  </si>
-  <si>
     <t>PK: record_id</t>
   </si>
   <si>
@@ -1189,15 +1186,6 @@
     <t>FK: record_type</t>
   </si>
   <si>
-    <t>Planner</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Record_type</t>
-  </si>
-  <si>
     <t>PK: Location_id</t>
   </si>
   <si>
@@ -1234,18 +1222,12 @@
     <t>quarter</t>
   </si>
   <si>
-    <t>Project descriptions</t>
-  </si>
-  <si>
     <t>planning_id</t>
   </si>
   <si>
     <t>for easier binning</t>
   </si>
   <si>
-    <t>Land use</t>
-  </si>
-  <si>
     <t>PK: land_use_id</t>
   </si>
   <si>
@@ -1255,18 +1237,9 @@
     <t>FK: record_id</t>
   </si>
   <si>
-    <t>Project Features</t>
-  </si>
-  <si>
-    <t>PK: prj_feature_id</t>
-  </si>
-  <si>
     <t>feature_type</t>
   </si>
   <si>
-    <t>Dwelling units</t>
-  </si>
-  <si>
     <t>PK: dwelling_id</t>
   </si>
   <si>
@@ -1276,12 +1249,6 @@
     <t>PK: prj_desc_id</t>
   </si>
   <si>
-    <t>year*</t>
-  </si>
-  <si>
-    <t>month*</t>
-  </si>
-  <si>
     <t>*violates 3NF, maybe remove?</t>
   </si>
   <si>
@@ -1300,9 +1267,6 @@
     <t>might be better just to have a separate database for each retrieval</t>
   </si>
   <si>
-    <t>details (for mcd/env)</t>
-  </si>
-  <si>
     <t>which I think makes sense because most of these attributes are sparse</t>
   </si>
   <si>
@@ -1399,12 +1363,6 @@
     <t>&lt;10% of all PRJ records, and 2% of all records.  More typically about 0.2%</t>
   </si>
   <si>
-    <t>quarter*</t>
-  </si>
-  <si>
-    <t>Entity</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -1489,9 +1447,6 @@
     <t>key for records</t>
   </si>
   <si>
-    <t>MCD_REFERRAL and ENVIRONMENTAL_REVIEW_TYPE have categoricals instead of just "checked or unchecked".  Sparsity is still about 1% so I'm putting them here.</t>
-  </si>
-  <si>
     <t>name of checkbox that got checked (e.g. "CHANGE_OF_USE", "ADDITIONS", "NEW_CONSTRUCTION")</t>
   </si>
   <si>
@@ -1534,24 +1489,12 @@
     <t>Property of what entity?</t>
   </si>
   <si>
-    <t>year of date_opened - calculated</t>
-  </si>
-  <si>
-    <t>quarter (1-4) of date_opened - calculated</t>
-  </si>
-  <si>
-    <t>month of date_opened - calculated</t>
-  </si>
-  <si>
     <t>For further explanation of these fields, see next sheet.</t>
   </si>
   <si>
     <t>An address for this location.  The format of these is extremely inconsistent, and sometimes a single building actually has two addresses.  I'll just pick one and drop the rest.</t>
   </si>
   <si>
-    <t>Record_rel</t>
-  </si>
-  <si>
     <t>PK: rel_id</t>
   </si>
   <si>
@@ -1636,18 +1579,12 @@
     <t>related_building_permit</t>
   </si>
   <si>
-    <t>mcd/env details</t>
-  </si>
-  <si>
     <t>Key for project descriptions. This table contains the subset of project descriptions which contain additional details</t>
   </si>
   <si>
     <t>MCD_REFERRAL and ENVIRONMENTAL_REVIEW_TYPE have categoricals instead of just "checked or unchecked".</t>
   </si>
   <si>
-    <t>ADU area</t>
-  </si>
-  <si>
     <t>key for dwelling unit changes</t>
   </si>
   <si>
@@ -1697,6 +1634,36 @@
   </si>
   <si>
     <t>prj_desc_detail</t>
+  </si>
+  <si>
+    <t>year_opened</t>
+  </si>
+  <si>
+    <t>month_opened</t>
+  </si>
+  <si>
+    <t>day_opened</t>
+  </si>
+  <si>
+    <t>year_closed</t>
+  </si>
+  <si>
+    <t>month_closed</t>
+  </si>
+  <si>
+    <t>day_closed</t>
+  </si>
+  <si>
+    <t>construct_cost</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>PK: feature_id</t>
+  </si>
+  <si>
+    <t>PK: desc_id</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1930,11 +1897,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1991,7 +1971,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2015,6 +1994,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2325,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2328,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="26" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="25"/>
@@ -2379,8 +2362,8 @@
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
-      <c r="G3" s="37" t="s">
-        <v>513</v>
+      <c r="G3" s="36" t="s">
+        <v>494</v>
       </c>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
@@ -2389,59 +2372,59 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" s="27"/>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>337</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="35" t="s">
-        <v>507</v>
+      <c r="G4" s="34" t="s">
+        <v>488</v>
       </c>
       <c r="H4" s="27"/>
       <c r="I4" s="20" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
       <c r="K4" s="27"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>376</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="35" t="s">
-        <v>382</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>546</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>545</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>508</v>
+      <c r="C5" s="43"/>
+      <c r="D5" s="34" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>525</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>524</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>489</v>
       </c>
       <c r="H5" s="27"/>
       <c r="I5" s="20" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="K5" s="27"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
-        <v>389</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>542</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>384</v>
+      <c r="B6" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>521</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>383</v>
       </c>
       <c r="E6" s="26"/>
-      <c r="F6" s="41" t="s">
-        <v>545</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>509</v>
+      <c r="F6" s="40" t="s">
+        <v>524</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>490</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -2449,15 +2432,15 @@
       <c r="L6" s="27"/>
     </row>
     <row r="7" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>331</v>
       </c>
       <c r="C7" s="27"/>
-      <c r="D7" s="36" t="s">
-        <v>402</v>
+      <c r="D7" s="35" t="s">
+        <v>397</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="42"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
@@ -2465,17 +2448,17 @@
       <c r="L7" s="27"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
-        <v>543</v>
+      <c r="B8" s="35" t="s">
+        <v>522</v>
       </c>
       <c r="C8" s="27"/>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="27"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="37" t="s">
-        <v>549</v>
+      <c r="F8" s="41"/>
+      <c r="G8" s="36" t="s">
+        <v>528</v>
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
@@ -2483,16 +2466,16 @@
       <c r="L8" s="27"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>379</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="35" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="27"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="35" t="s">
-        <v>405</v>
+      <c r="F9" s="41"/>
+      <c r="G9" s="34" t="s">
+        <v>399</v>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
@@ -2500,19 +2483,19 @@
       <c r="L9" s="27"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="32" t="s">
         <v>377</v>
       </c>
       <c r="C10" s="27"/>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="F10" s="43" t="s">
-        <v>545</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>407</v>
+      <c r="F10" s="42" t="s">
+        <v>524</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>401</v>
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
@@ -2521,13 +2504,13 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11" s="27"/>
-      <c r="D11" s="36" t="s">
-        <v>8</v>
+      <c r="D11" s="35" t="s">
+        <v>541</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="36" t="s">
-        <v>406</v>
+      <c r="F11" s="41"/>
+      <c r="G11" s="35" t="s">
+        <v>400</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
@@ -2535,17 +2518,17 @@
       <c r="L11" s="27"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="27"/>
-      <c r="D12" s="36" t="s">
-        <v>12</v>
+      <c r="D12" s="35" t="s">
+        <v>515</v>
       </c>
       <c r="E12" s="27"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="36" t="s">
-        <v>518</v>
+      <c r="F12" s="41"/>
+      <c r="G12" s="35" t="s">
+        <v>499</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
@@ -2553,19 +2536,19 @@
       <c r="L12" s="27"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>391</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>542</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>385</v>
+      <c r="B13" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>384</v>
       </c>
       <c r="E13" s="27"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="36" t="s">
-        <v>519</v>
+      <c r="F13" s="41"/>
+      <c r="G13" s="35" t="s">
+        <v>500</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -2573,17 +2556,17 @@
       <c r="L13" s="27"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
-        <v>394</v>
+      <c r="B14" s="35" t="s">
+        <v>390</v>
       </c>
       <c r="C14" s="27"/>
-      <c r="D14" s="36" t="s">
-        <v>2</v>
+      <c r="D14" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="E14" s="27"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="33" t="s">
-        <v>520</v>
+      <c r="F14" s="41"/>
+      <c r="G14" s="32" t="s">
+        <v>501</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
@@ -2591,15 +2574,15 @@
       <c r="L14" s="27"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="27"/>
-      <c r="D15" s="36" t="s">
-        <v>316</v>
+      <c r="D15" s="35" t="s">
+        <v>42</v>
       </c>
       <c r="E15" s="25"/>
-      <c r="F15" s="42"/>
+      <c r="F15" s="41"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
@@ -2607,16 +2590,16 @@
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>40</v>
+      <c r="D16" s="48" t="s">
+        <v>535</v>
       </c>
       <c r="E16" s="27"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="37" t="s">
-        <v>550</v>
+      <c r="F16" s="41"/>
+      <c r="G16" s="36" t="s">
+        <v>529</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
@@ -2625,13 +2608,13 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C17" s="27"/>
-      <c r="D17" s="36" t="s">
-        <v>42</v>
+      <c r="D17" s="48" t="s">
+        <v>536</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="35" t="s">
-        <v>409</v>
+      <c r="F17" s="41"/>
+      <c r="G17" s="34" t="s">
+        <v>543</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
@@ -2639,82 +2622,84 @@
       <c r="L17" s="27"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>338</v>
       </c>
       <c r="C18" s="27"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>537</v>
+      </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="30" t="s">
-        <v>545</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>407</v>
+      <c r="F18" s="29" t="s">
+        <v>524</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>401</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
-        <v>390</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>541</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>383</v>
+      <c r="B19" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>382</v>
       </c>
       <c r="E19" s="27"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="36" t="s">
-        <v>410</v>
+      <c r="F19" s="41"/>
+      <c r="G19" s="35" t="s">
+        <v>402</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
-        <v>392</v>
+      <c r="B20" s="35" t="s">
+        <v>388</v>
       </c>
       <c r="C20" s="27"/>
-      <c r="D20" s="36" t="s">
-        <v>415</v>
+      <c r="D20" s="35" t="s">
+        <v>538</v>
       </c>
       <c r="E20" s="27"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="36" t="s">
-        <v>521</v>
+      <c r="F20" s="41"/>
+      <c r="G20" s="35" t="s">
+        <v>502</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>456</v>
+      <c r="D21" s="35" t="s">
+        <v>539</v>
       </c>
       <c r="E21" s="27"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="36" t="s">
-        <v>522</v>
+      <c r="F21" s="41"/>
+      <c r="G21" s="35" t="s">
+        <v>503</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
-        <v>393</v>
+      <c r="B22" s="35" t="s">
+        <v>389</v>
       </c>
       <c r="C22" s="27"/>
-      <c r="D22" s="33" t="s">
-        <v>416</v>
+      <c r="D22" s="32" t="s">
+        <v>540</v>
       </c>
       <c r="E22" s="27"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="33" t="s">
-        <v>523</v>
+      <c r="F22" s="41"/>
+      <c r="G22" s="32" t="s">
+        <v>504</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="26"/>
@@ -2722,13 +2707,13 @@
       <c r="L22" s="27"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="42"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="26"/>
@@ -2740,13 +2725,13 @@
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="37" t="s">
-        <v>551</v>
+      <c r="F24" s="41"/>
+      <c r="G24" s="36" t="s">
+        <v>530</v>
       </c>
       <c r="H24" s="27"/>
-      <c r="I24" s="31" t="s">
-        <v>527</v>
+      <c r="I24" s="30" t="s">
+        <v>508</v>
       </c>
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
@@ -2755,35 +2740,35 @@
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="29" t="s">
-        <v>412</v>
-      </c>
-      <c r="H25" s="40" t="s">
-        <v>544</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>412</v>
+      <c r="F25" s="41"/>
+      <c r="G25" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>523</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>403</v>
       </c>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
-        <v>504</v>
-      </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
+      <c r="B26" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>407</v>
+        <v>524</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>401</v>
       </c>
       <c r="H26" s="27"/>
-      <c r="I26" s="30" t="s">
-        <v>527</v>
+      <c r="I26" s="29" t="s">
+        <v>508</v>
       </c>
       <c r="J26" s="27"/>
       <c r="K26" s="26"/>
@@ -2796,9 +2781,9 @@
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="36" t="s">
-        <v>413</v>
+      <c r="F27" s="45"/>
+      <c r="G27" s="35" t="s">
+        <v>404</v>
       </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
@@ -2811,9 +2796,9 @@
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="36" t="s">
-        <v>524</v>
+      <c r="F28" s="45"/>
+      <c r="G28" s="35" t="s">
+        <v>505</v>
       </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
@@ -2822,15 +2807,15 @@
       <c r="N28" s="27"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
-        <v>417</v>
-      </c>
-      <c r="C29" s="28"/>
+      <c r="B29" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="C29" s="47"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="36" t="s">
-        <v>525</v>
+      <c r="F29" s="45"/>
+      <c r="G29" s="35" t="s">
+        <v>506</v>
       </c>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
@@ -2840,9 +2825,9 @@
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="33" t="s">
-        <v>526</v>
+      <c r="F30" s="41"/>
+      <c r="G30" s="32" t="s">
+        <v>507</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
@@ -2854,7 +2839,7 @@
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="42"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
@@ -2864,42 +2849,42 @@
       <c r="O31" s="26"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="46"/>
-      <c r="G32" s="34" t="s">
-        <v>552</v>
-      </c>
-      <c r="I32" s="31" t="s">
-        <v>555</v>
+      <c r="F32" s="45"/>
+      <c r="G32" s="33" t="s">
+        <v>531</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>534</v>
       </c>
       <c r="L32" s="27"/>
       <c r="M32" s="27"/>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F33" s="46"/>
-      <c r="G33" s="29" t="s">
-        <v>414</v>
-      </c>
-      <c r="H33" s="30" t="s">
+      <c r="F33" s="45"/>
+      <c r="G33" s="28" t="s">
         <v>544</v>
       </c>
-      <c r="I33" s="29" t="s">
-        <v>414</v>
+      <c r="H33" s="29" t="s">
+        <v>523</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="I34" s="30" t="s">
-        <v>554</v>
+        <v>524</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="G35" s="33" t="s">
-        <v>421</v>
+      <c r="G35" s="32" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -2914,10 +2899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,797 +2912,789 @@
     <col min="3" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>457</v>
+        <v>542</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="C2" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="D2" t="s">
         <v>334</v>
       </c>
       <c r="E2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C3" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="D3" t="s">
         <v>334</v>
       </c>
       <c r="E3" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C4" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="D4" t="s">
         <v>334</v>
       </c>
       <c r="E4" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C5" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="D5" t="s">
         <v>335</v>
       </c>
       <c r="E5" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D6" t="s">
         <v>335</v>
       </c>
       <c r="E6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" t="s">
+        <v>457</v>
+      </c>
+      <c r="J8" t="s">
         <v>336</v>
       </c>
-      <c r="E8" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
+        <v>335</v>
+      </c>
+      <c r="E9" t="s">
+        <v>453</v>
+      </c>
+      <c r="J9" t="s">
         <v>336</v>
       </c>
-      <c r="E9" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>541</v>
       </c>
       <c r="D10" t="s">
-        <v>335</v>
+        <v>359</v>
       </c>
       <c r="E10" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>515</v>
       </c>
       <c r="D11" t="s">
         <v>335</v>
       </c>
       <c r="E11" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
         <v>335</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>535</v>
       </c>
       <c r="D14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>534</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>536</v>
       </c>
       <c r="D15" t="s">
-        <v>335</v>
-      </c>
-      <c r="E15" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>398</v>
+        <v>537</v>
       </c>
       <c r="D16" t="s">
         <v>334</v>
       </c>
-      <c r="E16" t="s">
-        <v>501</v>
-      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>400</v>
+        <v>538</v>
       </c>
       <c r="D17" t="s">
         <v>334</v>
       </c>
       <c r="E17" t="s">
-        <v>502</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>399</v>
+      <c r="B18" s="3" t="s">
+        <v>539</v>
       </c>
       <c r="D18" t="s">
         <v>334</v>
       </c>
-      <c r="E18" t="s">
-        <v>503</v>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="D19" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="50"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>338</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="C20" t="s">
-        <v>462</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C21" t="s">
+        <v>448</v>
+      </c>
+      <c r="D21" t="s">
         <v>334</v>
       </c>
-      <c r="E20" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="D21" t="s">
-        <v>335</v>
-      </c>
       <c r="E21" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>388</v>
       </c>
       <c r="D22" t="s">
         <v>335</v>
       </c>
       <c r="E22" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>393</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>335</v>
       </c>
       <c r="E23" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>38</v>
+      <c r="B24" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D24" t="s">
         <v>335</v>
       </c>
       <c r="E24" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C26" t="s">
-        <v>462</v>
-      </c>
-      <c r="D26" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
         <v>335</v>
       </c>
-      <c r="E26" t="s">
-        <v>480</v>
+      <c r="E25" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>394</v>
+      <c r="A27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C27" t="s">
+        <v>448</v>
       </c>
       <c r="D27" t="s">
         <v>335</v>
       </c>
       <c r="E27" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>528</v>
+        <v>390</v>
       </c>
       <c r="D28" t="s">
         <v>335</v>
       </c>
       <c r="E28" t="s">
-        <v>530</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>529</v>
+      <c r="B29" s="3" t="s">
+        <v>509</v>
       </c>
       <c r="D29" t="s">
         <v>335</v>
       </c>
       <c r="E29" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C31" t="s">
-        <v>462</v>
-      </c>
-      <c r="D31" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D30" t="s">
+        <v>335</v>
+      </c>
+      <c r="E30" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C32" t="s">
+        <v>448</v>
+      </c>
+      <c r="D32" t="s">
         <v>334</v>
       </c>
-      <c r="E31" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="D32" t="s">
-        <v>335</v>
-      </c>
       <c r="E32" t="s">
-        <v>481</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>331</v>
       </c>
       <c r="D33" t="s">
         <v>335</v>
       </c>
       <c r="E33" t="s">
-        <v>505</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>532</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="E34" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>533</v>
+      <c r="B35" s="3" t="s">
+        <v>513</v>
       </c>
       <c r="D35" t="s">
         <v>359</v>
       </c>
       <c r="E35" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C37" t="s">
-        <v>462</v>
-      </c>
-      <c r="D37" t="s">
-        <v>334</v>
-      </c>
-      <c r="E37" t="s">
-        <v>484</v>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="D36" t="s">
+        <v>359</v>
+      </c>
+      <c r="E36" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>407</v>
+      <c r="A38" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>544</v>
       </c>
       <c r="C38" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="D38" t="s">
         <v>334</v>
       </c>
       <c r="E38" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>421</v>
+        <v>401</v>
+      </c>
+      <c r="C39" t="s">
+        <v>449</v>
       </c>
       <c r="D39" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E39" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>423</v>
+      <c r="B40" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="D40" t="s">
         <v>335</v>
       </c>
       <c r="E40" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="C42" t="s">
-        <v>462</v>
-      </c>
-      <c r="D42" t="s">
-        <v>334</v>
-      </c>
-      <c r="E42" t="s">
-        <v>492</v>
-      </c>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="8"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>407</v>
+      <c r="A43" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>399</v>
       </c>
       <c r="C43" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="D43" t="s">
         <v>334</v>
       </c>
       <c r="E43" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
+      </c>
+      <c r="C44" t="s">
+        <v>449</v>
       </c>
       <c r="D44" t="s">
+        <v>334</v>
+      </c>
+      <c r="E44" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D45" t="s">
         <v>335</v>
       </c>
-      <c r="E44" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="D45" t="s">
-        <v>359</v>
-      </c>
       <c r="E45" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="D46" t="s">
         <v>359</v>
       </c>
       <c r="E46" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
-        <v>520</v>
+      <c r="B47" s="6" t="s">
+        <v>500</v>
       </c>
       <c r="D47" t="s">
         <v>359</v>
       </c>
       <c r="E47" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C49" t="s">
-        <v>462</v>
-      </c>
-      <c r="D49" t="s">
-        <v>334</v>
-      </c>
-      <c r="E49" t="s">
-        <v>493</v>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="D48" t="s">
+        <v>359</v>
+      </c>
+      <c r="E48" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>407</v>
+      <c r="A50" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>543</v>
       </c>
       <c r="C50" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="D50" t="s">
         <v>334</v>
       </c>
       <c r="E50" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>410</v>
+        <v>401</v>
+      </c>
+      <c r="C51" t="s">
+        <v>449</v>
       </c>
       <c r="D51" t="s">
+        <v>334</v>
+      </c>
+      <c r="E51" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="D52" t="s">
         <v>335</v>
       </c>
-      <c r="E51" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="D52" t="s">
-        <v>334</v>
-      </c>
       <c r="E52" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
       <c r="D53" t="s">
         <v>334</v>
       </c>
       <c r="E53" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
-        <v>523</v>
+      <c r="B54" s="6" t="s">
+        <v>503</v>
       </c>
       <c r="D54" t="s">
         <v>334</v>
       </c>
       <c r="E54" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C56" t="s">
-        <v>462</v>
-      </c>
-      <c r="D56" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="D55" t="s">
         <v>334</v>
       </c>
-      <c r="E56" t="s">
-        <v>497</v>
+      <c r="E55" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>407</v>
+      <c r="A57" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>403</v>
       </c>
       <c r="C57" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="D57" t="s">
         <v>334</v>
       </c>
       <c r="E57" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>413</v>
+        <v>401</v>
+      </c>
+      <c r="C58" t="s">
+        <v>449</v>
       </c>
       <c r="D58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E58" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>524</v>
+        <v>404</v>
       </c>
       <c r="D59" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E59" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="D60" t="s">
         <v>334</v>
       </c>
       <c r="E60" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="6" t="s">
-        <v>526</v>
+      <c r="B61" s="3" t="s">
+        <v>506</v>
       </c>
       <c r="D61" t="s">
         <v>334</v>
       </c>
       <c r="E61" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>527</v>
+      <c r="B62" s="6" t="s">
+        <v>507</v>
       </c>
       <c r="D62" t="s">
-        <v>359</v>
+        <v>334</v>
       </c>
       <c r="E62" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="C64" t="s">
-        <v>462</v>
-      </c>
-      <c r="D64" t="s">
-        <v>334</v>
-      </c>
-      <c r="E64" t="s">
-        <v>512</v>
-      </c>
-    </row>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="12" t="s">
-        <v>508</v>
+      <c r="A65" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>488</v>
       </c>
       <c r="C65" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="D65" t="s">
         <v>334</v>
       </c>
       <c r="E65" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="13" t="s">
-        <v>509</v>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="12" t="s">
+        <v>489</v>
       </c>
       <c r="C66" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="D66" t="s">
         <v>334</v>
       </c>
       <c r="E66" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
-        <v>535</v>
-      </c>
-      <c r="B68" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>462</v>
-      </c>
-      <c r="D68" s="19" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C67" t="s">
+        <v>449</v>
+      </c>
+      <c r="D67" t="s">
         <v>334</v>
       </c>
-      <c r="E68" s="20" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="22" t="s">
-        <v>554</v>
-      </c>
-      <c r="C69" s="19"/>
+      <c r="E67" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>448</v>
+      </c>
       <c r="D69" s="19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>537</v>
+        <v>516</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
-      <c r="B70" s="19"/>
+      <c r="B70" s="22" t="s">
+        <v>533</v>
+      </c>
       <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
-        <v>538</v>
-      </c>
-      <c r="B71" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>462</v>
-      </c>
-      <c r="D71" s="19" t="s">
+      <c r="A71" s="19"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="23" t="s">
+        <v>508</v>
+      </c>
+      <c r="B72" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="D72" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="E71" s="20" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
-      <c r="B72" s="22" t="s">
-        <v>540</v>
-      </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19" t="s">
+      <c r="E72" s="20" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="19"/>
+      <c r="B73" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="E72" s="20" t="s">
-        <v>499</v>
+      <c r="E73" s="20" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -3730,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3747,7 +3724,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3759,10 +3736,10 @@
         <v>362</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>330</v>
@@ -3817,7 +3794,7 @@
         <v>347</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3838,10 +3815,10 @@
         <v>337</v>
       </c>
       <c r="G5" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="H5" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3880,7 +3857,7 @@
         <v>337</v>
       </c>
       <c r="G7" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3901,7 +3878,7 @@
         <v>337</v>
       </c>
       <c r="G8" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3922,7 +3899,7 @@
         <v>376</v>
       </c>
       <c r="G9" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3943,7 +3920,7 @@
         <v>342</v>
       </c>
       <c r="G10" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3964,7 +3941,7 @@
         <v>342</v>
       </c>
       <c r="G11" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4057,7 +4034,7 @@
         <v>337</v>
       </c>
       <c r="H16" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4099,7 +4076,7 @@
         <v>338</v>
       </c>
       <c r="H18" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4138,7 +4115,7 @@
         <v>347</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4155,16 +4132,16 @@
         <v>334</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>514</v>
+        <v>495</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4181,16 +4158,16 @@
         <v>334</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>516</v>
+        <v>497</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4211,10 +4188,10 @@
         <v>337</v>
       </c>
       <c r="F23" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="G23" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4235,7 +4212,7 @@
         <v>338</v>
       </c>
       <c r="G24" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4256,7 +4233,7 @@
         <v>338</v>
       </c>
       <c r="G25" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4277,7 +4254,7 @@
         <v>338</v>
       </c>
       <c r="G26" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4327,13 +4304,13 @@
         <v>337</v>
       </c>
       <c r="F30" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="G30" t="s">
         <v>357</v>
       </c>
       <c r="H30" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4348,7 +4325,7 @@
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4363,7 +4340,7 @@
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -4390,7 +4367,7 @@
         <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4456,7 +4433,7 @@
         <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4471,7 +4448,7 @@
         <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -4498,7 +4475,7 @@
         <v>67</v>
       </c>
       <c r="F42" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -4624,7 +4601,7 @@
         <v>340</v>
       </c>
       <c r="F52" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H52" t="s">
         <v>356</v>
@@ -4657,7 +4634,7 @@
         <v>340</v>
       </c>
       <c r="F54" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="H54" t="s">
         <v>358</v>
@@ -4668,13 +4645,13 @@
         <v>360</v>
       </c>
       <c r="D56" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="E56" t="s">
         <v>354</v>
       </c>
       <c r="F56" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="G56" t="s">
         <v>366</v>
@@ -4979,7 +4956,7 @@
         <v>354</v>
       </c>
       <c r="F82" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="G82" t="s">
         <v>366</v>
@@ -5135,7 +5112,7 @@
         <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>553</v>
+        <v>532</v>
       </c>
       <c r="C95" t="s">
         <v>165</v>
@@ -5153,7 +5130,7 @@
         <v>167</v>
       </c>
       <c r="G96" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -5228,7 +5205,7 @@
         <v>178</v>
       </c>
       <c r="G102" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -5435,10 +5412,10 @@
         <v>211</v>
       </c>
       <c r="F119" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="H119" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5453,7 +5430,7 @@
         <v>213</v>
       </c>
       <c r="F120" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5468,7 +5445,7 @@
         <v>215</v>
       </c>
       <c r="F121" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5483,7 +5460,7 @@
         <v>217</v>
       </c>
       <c r="F122" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5498,7 +5475,7 @@
         <v>219</v>
       </c>
       <c r="F123" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5513,7 +5490,7 @@
         <v>221</v>
       </c>
       <c r="F124" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5528,7 +5505,7 @@
         <v>223</v>
       </c>
       <c r="F125" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5543,7 +5520,7 @@
         <v>225</v>
       </c>
       <c r="F126" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5558,7 +5535,7 @@
         <v>227</v>
       </c>
       <c r="F127" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5576,10 +5553,10 @@
         <v>335</v>
       </c>
       <c r="F128" s="18" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="G128" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
       <c r="H128" s="18" t="s">
         <v>364</v>
@@ -5635,7 +5612,7 @@
         <v>354</v>
       </c>
       <c r="F133" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="G133" t="s">
         <v>366</v>
@@ -5836,7 +5813,7 @@
         <v>359</v>
       </c>
       <c r="H149" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -5890,7 +5867,7 @@
         <v>359</v>
       </c>
       <c r="H153" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -5944,7 +5921,7 @@
         <v>359</v>
       </c>
       <c r="H157" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -5998,7 +5975,7 @@
         <v>359</v>
       </c>
       <c r="H161" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -6121,7 +6098,7 @@
         <v>311</v>
       </c>
       <c r="F171" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -6136,7 +6113,7 @@
         <v>313</v>
       </c>
       <c r="F172" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -6151,7 +6128,7 @@
         <v>315</v>
       </c>
       <c r="F173" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -6177,13 +6154,13 @@
         <v>337</v>
       </c>
       <c r="F176" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="G176" t="s">
         <v>368</v>
       </c>
       <c r="H176" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
     </row>
     <row r="177" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6198,7 +6175,7 @@
         <v>319</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="G177" s="9" t="s">
         <v>347</v>
@@ -6219,7 +6196,7 @@
         <v>321</v>
       </c>
       <c r="F178" s="9" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="G178" s="9" t="s">
         <v>347</v>
@@ -6237,7 +6214,7 @@
         <v>323</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="G179" s="9" t="s">
         <v>347</v>
@@ -6258,10 +6235,10 @@
         <v>371</v>
       </c>
       <c r="F180" s="9" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G180" s="9" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="H180" s="9" t="s">
         <v>370</v>
@@ -6282,10 +6259,10 @@
         <v>371</v>
       </c>
       <c r="F181" s="9" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G181" s="9" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="H181" s="9" t="s">
         <v>370</v>
@@ -6306,10 +6283,10 @@
         <v>371</v>
       </c>
       <c r="F182" s="9" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G182" s="9" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="H182" s="9" t="s">
         <v>372</v>
@@ -6353,15 +6330,15 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C186" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C187" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D187" t="s">
         <v>334</v>
@@ -6370,15 +6347,15 @@
         <v>337</v>
       </c>
       <c r="H187" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C188" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D188" t="s">
         <v>334</v>
@@ -6389,10 +6366,10 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C189" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D189" t="s">
         <v>334</v>
@@ -6403,21 +6380,21 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="C190" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="D190" t="s">
         <v>336</v>
       </c>
       <c r="H190" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H191" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make column names adjustable, add unit tests
</commit_message>
<xml_diff>
--- a/Database structure.xlsx
+++ b/Database structure.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="545">
   <si>
     <t>Field</t>
   </si>
@@ -1156,60 +1156,18 @@
     <t>Shape_Length</t>
   </si>
   <si>
-    <t>PK: record_id</t>
-  </si>
-  <si>
-    <t>FK: planner_id</t>
-  </si>
-  <si>
-    <t>FK: location_id</t>
-  </si>
-  <si>
-    <t>FK: record_type</t>
-  </si>
-  <si>
-    <t>PK: Location_id</t>
-  </si>
-  <si>
-    <t>PK: Planner_id</t>
-  </si>
-  <si>
-    <t>PK: record_type</t>
-  </si>
-  <si>
-    <t>planner_strid</t>
-  </si>
-  <si>
-    <t>planner_e-mail</t>
-  </si>
-  <si>
-    <t>record_type_name</t>
-  </si>
-  <si>
     <t>Database schema</t>
   </si>
   <si>
-    <t>PK: land_use_id</t>
-  </si>
-  <si>
     <t>land_use_type</t>
   </si>
   <si>
-    <t>FK: record_id</t>
-  </si>
-  <si>
     <t>feature_type</t>
   </si>
   <si>
     <t>PK: dwelling_id</t>
   </si>
   <si>
-    <t>dwelling_type</t>
-  </si>
-  <si>
-    <t>PK: prj_desc_id</t>
-  </si>
-  <si>
     <t>*violates 3NF, maybe remove?</t>
   </si>
   <si>
@@ -1444,42 +1402,9 @@
     <t>type of project feature (e.g. affordable units, market units, parking spaces).  For "other" features, the name of the feature will be listed here if available.</t>
   </si>
   <si>
-    <t>land_use_exist</t>
-  </si>
-  <si>
-    <t>land_use_prop</t>
-  </si>
-  <si>
-    <t>land_use_net*</t>
-  </si>
-  <si>
-    <t>feature_exist</t>
-  </si>
-  <si>
-    <t>feature_prop</t>
-  </si>
-  <si>
-    <t>feature_net*</t>
-  </si>
-  <si>
-    <t>dwelling_exist</t>
-  </si>
-  <si>
-    <t>dwelling_prop</t>
-  </si>
-  <si>
-    <t>dwelling_net*</t>
-  </si>
-  <si>
     <t>adu_area</t>
   </si>
   <si>
-    <t>record_type_subcat</t>
-  </si>
-  <si>
-    <t>record_type_cat</t>
-  </si>
-  <si>
     <t>One of 17 subcategories of records (e.g. Environmental, Referrals, Legislation)</t>
   </si>
   <si>
@@ -1576,15 +1501,9 @@
     <t>Table</t>
   </si>
   <si>
-    <t>PK: feature_id</t>
-  </si>
-  <si>
     <t>PK: desc_id</t>
   </si>
   <si>
-    <t>PK: record_index</t>
-  </si>
-  <si>
     <t>A key being created for this database.  I would have called it record_id, but there's already a variable under that name</t>
   </si>
   <si>
@@ -1624,9 +1543,6 @@
     <t>calculated from date_closed</t>
   </si>
   <si>
-    <t>record_strid</t>
-  </si>
-  <si>
     <t>In this data, always "planning", but hypothetically we could add data from other departments to the database</t>
   </si>
   <si>
@@ -1651,9 +1567,6 @@
     <t>key for BOS hearing dates, as well as mayoral signings.</t>
   </si>
   <si>
-    <t>PK: hearing_id</t>
-  </si>
-  <si>
     <t>MCD_REFERRAL and ENVIRONMENTAL_REVIEW_TYPE</t>
   </si>
   <si>
@@ -1693,10 +1606,64 @@
     <t>prj_desc_details</t>
   </si>
   <si>
-    <t>Shape_length</t>
-  </si>
-  <si>
-    <t>Shape_area</t>
+    <t>PK: id</t>
+  </si>
+  <si>
+    <t>PK: location_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>PK: category</t>
+  </si>
+  <si>
+    <t>subtype</t>
+  </si>
+  <si>
+    <t>FK: record</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>exist</t>
+  </si>
+  <si>
+    <t>prop</t>
+  </si>
+  <si>
+    <t>*net</t>
+  </si>
+  <si>
+    <t>net*</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>FK: planner</t>
+  </si>
+  <si>
+    <t>FK: location</t>
+  </si>
+  <si>
+    <t>FK: category</t>
+  </si>
+  <si>
+    <t>FK: parent</t>
+  </si>
+  <si>
+    <t>FK: child</t>
+  </si>
+  <si>
+    <t>record_group</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +1983,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -2039,14 +2005,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2357,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,7 +2342,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="20" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="19"/>
@@ -2412,7 +2377,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="30" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
@@ -2427,11 +2392,11 @@
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
       <c r="G4" s="28" t="s">
-        <v>461</v>
+        <v>525</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="14" t="s">
-        <v>498</v>
+        <v>473</v>
       </c>
       <c r="K4" s="21"/>
     </row>
@@ -2441,39 +2406,39 @@
       </c>
       <c r="C5" s="37"/>
       <c r="D5" s="28" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>497</v>
+        <v>472</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>496</v>
+        <v>471</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>462</v>
+        <v>542</v>
       </c>
       <c r="H5" s="21"/>
       <c r="I5" s="14" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="K5" s="21"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>379</v>
+        <v>526</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>493</v>
+        <v>468</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>377</v>
+        <v>540</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="34" t="s">
-        <v>496</v>
+        <v>471</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>463</v>
+        <v>543</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
@@ -2498,16 +2463,16 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
-        <v>494</v>
+        <v>469</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="29" t="s">
-        <v>22</v>
+        <v>527</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="35"/>
       <c r="G8" s="30" t="s">
-        <v>500</v>
+        <v>475</v>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -2516,15 +2481,15 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
-        <v>374</v>
+        <v>460</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="35"/>
-      <c r="G9" s="28" t="s">
-        <v>386</v>
+      <c r="G9" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
@@ -2533,18 +2498,18 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>372</v>
+        <v>461</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="29" t="s">
-        <v>10</v>
+        <v>538</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="36" t="s">
-        <v>496</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>388</v>
+        <v>471</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>532</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -2554,12 +2519,12 @@
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11" s="21"/>
       <c r="D11" s="29" t="s">
-        <v>513</v>
+        <v>488</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="35"/>
-      <c r="G11" s="29" t="s">
-        <v>387</v>
+      <c r="G11" s="3" t="s">
+        <v>376</v>
       </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
@@ -2572,12 +2537,12 @@
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="29" t="s">
-        <v>487</v>
+        <v>462</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="35"/>
-      <c r="G12" s="29" t="s">
-        <v>471</v>
+      <c r="G12" s="6" t="s">
+        <v>534</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
@@ -2586,18 +2551,18 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>381</v>
+        <v>530</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>493</v>
+        <v>468</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>378</v>
+        <v>541</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="35"/>
-      <c r="G13" s="29" t="s">
-        <v>472</v>
+      <c r="G13" s="6" t="s">
+        <v>535</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -2605,8 +2570,8 @@
       <c r="L13" s="21"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
-        <v>384</v>
+      <c r="B14" s="3" t="s">
+        <v>527</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="29" t="s">
@@ -2614,8 +2579,8 @@
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="35"/>
-      <c r="G14" s="26" t="s">
-        <v>473</v>
+      <c r="G14" s="7" t="s">
+        <v>536</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
@@ -2623,8 +2588,8 @@
       <c r="L14" s="21"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
-        <v>19</v>
+      <c r="B15" s="3" t="s">
+        <v>531</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="29" t="s">
@@ -2639,16 +2604,16 @@
       <c r="L15" s="21"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="26" t="s">
-        <v>20</v>
+      <c r="B16" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>507</v>
+        <v>482</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="35"/>
       <c r="G16" s="30" t="s">
-        <v>501</v>
+        <v>476</v>
       </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
@@ -2656,14 +2621,17 @@
       <c r="L16" s="21"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>544</v>
+      </c>
       <c r="C17" s="21"/>
       <c r="D17" s="41" t="s">
-        <v>508</v>
+        <v>483</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="35"/>
-      <c r="G17" s="28" t="s">
-        <v>515</v>
+      <c r="G17" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
@@ -2671,84 +2639,81 @@
       <c r="L17" s="21"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="30" t="s">
-        <v>337</v>
+      <c r="B18" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="3" t="s">
-        <v>509</v>
+        <v>484</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>388</v>
+        <v>471</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>532</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
-        <v>380</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>492</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>376</v>
+      <c r="D19" s="29" t="s">
+        <v>485</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="35"/>
-      <c r="G19" s="29" t="s">
-        <v>389</v>
+      <c r="G19" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
-        <v>382</v>
+      <c r="B20" s="30" t="s">
+        <v>337</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="29" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="29" t="s">
-        <v>474</v>
+      <c r="G20" s="6" t="s">
+        <v>534</v>
       </c>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>511</v>
+      <c r="B21" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>467</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>539</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="29" t="s">
-        <v>475</v>
+      <c r="G21" s="6" t="s">
+        <v>535</v>
       </c>
       <c r="H21" s="21"/>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
-        <v>383</v>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="29" t="s">
-        <v>512</v>
+        <v>487</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="26" t="s">
-        <v>476</v>
+      <c r="G22" s="7" t="s">
+        <v>537</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="20"/>
@@ -2756,12 +2721,12 @@
       <c r="L22" s="21"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
-        <v>38</v>
+      <c r="B23" s="3" t="s">
+        <v>527</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="6" t="s">
-        <v>520</v>
+        <v>493</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="35"/>
@@ -2772,56 +2737,55 @@
       <c r="L23" s="21"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
+      <c r="B24" s="3" t="s">
+        <v>528</v>
+      </c>
       <c r="C24" s="21"/>
       <c r="D24" s="7" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="35"/>
       <c r="G24" s="30" t="s">
-        <v>502</v>
+        <v>477</v>
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="24" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>529</v>
+      </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="35"/>
-      <c r="G25" s="22" t="s">
-        <v>390</v>
+      <c r="G25" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>495</v>
+        <v>470</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
-        <v>459</v>
-      </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
       <c r="F26" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>388</v>
+        <v>471</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>532</v>
       </c>
       <c r="H26" s="21"/>
       <c r="I26" s="23" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="J26" s="21"/>
       <c r="K26" s="20"/>
@@ -2830,13 +2794,15 @@
       <c r="N26" s="21"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="B27" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
       <c r="F27" s="39"/>
-      <c r="G27" s="29" t="s">
-        <v>391</v>
+      <c r="G27" s="3" t="s">
+        <v>533</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
@@ -2850,8 +2816,8 @@
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="39"/>
-      <c r="G28" s="29" t="s">
-        <v>477</v>
+      <c r="G28" s="3" t="s">
+        <v>534</v>
       </c>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
@@ -2860,15 +2826,15 @@
       <c r="N28" s="21"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
-        <v>393</v>
-      </c>
-      <c r="C29" s="44"/>
+      <c r="B29" s="55" t="s">
+        <v>379</v>
+      </c>
+      <c r="C29" s="55"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="39"/>
-      <c r="G29" s="29" t="s">
-        <v>478</v>
+      <c r="G29" s="3" t="s">
+        <v>535</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
@@ -2879,8 +2845,8 @@
       <c r="C30" s="21"/>
       <c r="E30" s="21"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="26" t="s">
-        <v>479</v>
+      <c r="G30" s="7" t="s">
+        <v>537</v>
       </c>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
@@ -2904,41 +2870,41 @@
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="39"/>
       <c r="G32" s="27" t="s">
-        <v>503</v>
+        <v>478</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33" s="39"/>
-      <c r="G33" s="22" t="s">
-        <v>516</v>
+      <c r="G33" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="H33" s="23" t="s">
-        <v>495</v>
-      </c>
-      <c r="I33" s="22" t="s">
-        <v>516</v>
+        <v>470</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>388</v>
-      </c>
-      <c r="I34" s="23" t="s">
-        <v>505</v>
+        <v>471</v>
+      </c>
+      <c r="G34" s="56" t="s">
+        <v>532</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F35" s="54"/>
-      <c r="G35" s="26" t="s">
-        <v>394</v>
+      <c r="F35" s="52"/>
+      <c r="G35" s="4" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.25">
@@ -2947,26 +2913,26 @@
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37" s="39"/>
       <c r="G37" s="2" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
     </row>
     <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38" s="39"/>
-      <c r="G38" s="51" t="s">
-        <v>540</v>
+      <c r="G38" s="50" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F39" s="55" t="s">
-        <v>496</v>
-      </c>
-      <c r="G39" s="56" t="s">
-        <v>388</v>
+      <c r="F39" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="G39" s="54" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="G40" s="6" t="s">
-        <v>535</v>
+        <v>507</v>
       </c>
     </row>
     <row r="41" spans="6:9" x14ac:dyDescent="0.25">
@@ -2976,7 +2942,7 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
     <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2988,8 +2954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD83"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,19 +2968,19 @@
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>514</v>
+        <v>489</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>527</v>
+        <v>500</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -3025,61 +2991,61 @@
         <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>375</v>
+        <v>525</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D2" t="s">
         <v>333</v>
       </c>
       <c r="E2" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F2" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>376</v>
+        <v>539</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D3" t="s">
         <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F3" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>377</v>
+        <v>540</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D4" t="s">
         <v>333</v>
       </c>
       <c r="E4" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F4" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>378</v>
+        <v>541</v>
       </c>
       <c r="C5" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D5" t="s">
         <v>334</v>
@@ -3088,26 +3054,23 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>531</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>334</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>520</v>
+        <v>493</v>
       </c>
       <c r="D7" t="s">
         <v>333</v>
@@ -3116,13 +3079,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
     </row>
     <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>334</v>
@@ -19514,13 +19477,16 @@
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>527</v>
       </c>
       <c r="D9" t="s">
         <v>334</v>
       </c>
+      <c r="E9" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
@@ -19531,7 +19497,7 @@
         <v>334</v>
       </c>
       <c r="F10" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="K10" t="s">
         <v>335</v>
@@ -19539,13 +19505,16 @@
     </row>
     <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>538</v>
       </c>
       <c r="D11" t="s">
         <v>334</v>
       </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
       <c r="F11" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="K11" t="s">
         <v>335</v>
@@ -19553,7 +19522,7 @@
     </row>
     <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>513</v>
+        <v>488</v>
       </c>
       <c r="D12" t="s">
         <v>356</v>
@@ -19567,7 +19536,7 @@
     </row>
     <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>487</v>
+        <v>462</v>
       </c>
       <c r="D13" t="s">
         <v>334</v>
@@ -19576,7 +19545,7 @@
         <v>316</v>
       </c>
       <c r="F13" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
@@ -19603,74 +19572,74 @@
     </row>
     <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>507</v>
+        <v>482</v>
       </c>
       <c r="D16" t="s">
         <v>333</v>
       </c>
       <c r="E16" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="F16" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>508</v>
+        <v>483</v>
       </c>
       <c r="D17" t="s">
         <v>333</v>
       </c>
       <c r="E17" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>509</v>
+        <v>484</v>
       </c>
       <c r="D18" t="s">
         <v>333</v>
       </c>
       <c r="E18" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>510</v>
+        <v>485</v>
       </c>
       <c r="D19" t="s">
         <v>333</v>
       </c>
       <c r="E19" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="F19" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>511</v>
+        <v>486</v>
       </c>
       <c r="D20" t="s">
         <v>333</v>
       </c>
       <c r="E20" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>512</v>
+        <v>487</v>
       </c>
       <c r="D21" t="s">
         <v>333</v>
       </c>
       <c r="E21" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -19681,66 +19650,72 @@
         <v>337</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>380</v>
+        <v>525</v>
       </c>
       <c r="C23" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D23" t="s">
         <v>333</v>
       </c>
       <c r="E23" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F23" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>382</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
         <v>334</v>
       </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
       <c r="F24" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>527</v>
       </c>
       <c r="D25" t="s">
         <v>334</v>
       </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
       <c r="F25" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>36</v>
+        <v>528</v>
       </c>
       <c r="D26" t="s">
         <v>334</v>
       </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
       <c r="F26" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>529</v>
       </c>
       <c r="D27" t="s">
         <v>334</v>
       </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
       <c r="F27" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -19748,10 +19723,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>381</v>
+        <v>530</v>
       </c>
       <c r="C29" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D29" t="s">
         <v>334</v>
@@ -19760,12 +19735,12 @@
         <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>384</v>
+        <v>527</v>
       </c>
       <c r="D30" t="s">
         <v>334</v>
@@ -19774,12 +19749,12 @@
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>481</v>
+        <v>531</v>
       </c>
       <c r="D31" t="s">
         <v>334</v>
@@ -19788,12 +19763,12 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>483</v>
+        <v>458</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>482</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
         <v>334</v>
@@ -19802,18 +19777,21 @@
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>484</v>
+        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>18</v>
+        <v>544</v>
       </c>
       <c r="D33" t="s">
         <v>334</v>
       </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
       <c r="F33" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -19824,7 +19802,7 @@
         <v>334</v>
       </c>
       <c r="F34" t="s">
-        <v>533</v>
+        <v>505</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -19832,19 +19810,19 @@
         <v>371</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>379</v>
+        <v>526</v>
       </c>
       <c r="C36" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D36" t="s">
         <v>333</v>
       </c>
       <c r="E36" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F36" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -19855,7 +19833,7 @@
         <v>334</v>
       </c>
       <c r="F37" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -19866,394 +19844,394 @@
         <v>334</v>
       </c>
       <c r="F38" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>485</v>
+        <v>460</v>
       </c>
       <c r="D39" t="s">
         <v>356</v>
       </c>
       <c r="E39" t="s">
-        <v>554</v>
+        <v>374</v>
       </c>
       <c r="F39" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>486</v>
+        <v>461</v>
       </c>
       <c r="D40" t="s">
         <v>356</v>
       </c>
       <c r="E40" t="s">
-        <v>555</v>
+        <v>372</v>
       </c>
       <c r="F40" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>503</v>
+        <v>478</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="C42" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D42" t="s">
         <v>333</v>
       </c>
       <c r="E42" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F42" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>388</v>
+        <v>532</v>
       </c>
       <c r="C43" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D43" t="s">
         <v>333</v>
       </c>
       <c r="E43" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F43" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="D44" t="s">
         <v>334</v>
       </c>
       <c r="E44" t="s">
-        <v>542</v>
+        <v>513</v>
       </c>
       <c r="F44" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>500</v>
+        <v>475</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>386</v>
+        <v>525</v>
       </c>
       <c r="C46" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D46" t="s">
         <v>333</v>
       </c>
       <c r="E46" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F46" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
-        <v>388</v>
+      <c r="B47" s="56" t="s">
+        <v>532</v>
       </c>
       <c r="C47" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D47" t="s">
         <v>333</v>
       </c>
       <c r="E47" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F47" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="D48" t="s">
         <v>334</v>
       </c>
       <c r="E48" t="s">
-        <v>543</v>
+        <v>514</v>
       </c>
       <c r="F48" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>471</v>
+        <v>534</v>
       </c>
       <c r="D49" t="s">
         <v>356</v>
       </c>
       <c r="E49" t="s">
-        <v>544</v>
+        <v>515</v>
       </c>
       <c r="F49" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
-        <v>472</v>
+        <v>535</v>
       </c>
       <c r="D50" t="s">
         <v>356</v>
       </c>
       <c r="E50" t="s">
-        <v>545</v>
+        <v>516</v>
       </c>
       <c r="F50" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
-        <v>473</v>
+        <v>536</v>
       </c>
       <c r="D51" t="s">
         <v>356</v>
       </c>
       <c r="E51" t="s">
-        <v>546</v>
+        <v>517</v>
       </c>
       <c r="F51" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>501</v>
+        <v>476</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="C53" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D53" t="s">
         <v>333</v>
       </c>
       <c r="E53" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F53" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>388</v>
+        <v>532</v>
       </c>
       <c r="C54" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D54" t="s">
         <v>333</v>
       </c>
       <c r="E54" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F54" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="D55" t="s">
         <v>334</v>
       </c>
       <c r="E55" t="s">
-        <v>547</v>
+        <v>518</v>
       </c>
       <c r="F55" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
-        <v>474</v>
+        <v>534</v>
       </c>
       <c r="D56" t="s">
         <v>333</v>
       </c>
       <c r="E56" t="s">
-        <v>547</v>
+        <v>518</v>
       </c>
       <c r="F56" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>475</v>
+        <v>535</v>
       </c>
       <c r="D57" t="s">
         <v>333</v>
       </c>
       <c r="E57" t="s">
-        <v>547</v>
+        <v>518</v>
       </c>
       <c r="F57" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="s">
-        <v>476</v>
+        <v>537</v>
       </c>
       <c r="D58" t="s">
         <v>333</v>
       </c>
       <c r="E58" t="s">
-        <v>547</v>
+        <v>518</v>
       </c>
       <c r="F58" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>502</v>
+        <v>477</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>390</v>
+        <v>525</v>
       </c>
       <c r="C60" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D60" t="s">
         <v>333</v>
       </c>
       <c r="E60" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F60" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>388</v>
+      <c r="B61" s="56" t="s">
+        <v>532</v>
       </c>
       <c r="C61" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D61" t="s">
         <v>333</v>
       </c>
       <c r="E61" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F61" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>391</v>
+        <v>533</v>
       </c>
       <c r="D62" t="s">
         <v>334</v>
       </c>
       <c r="E62" t="s">
-        <v>548</v>
+        <v>519</v>
       </c>
       <c r="F62" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>477</v>
+        <v>534</v>
       </c>
       <c r="D63" t="s">
         <v>333</v>
       </c>
       <c r="E63" t="s">
-        <v>548</v>
+        <v>519</v>
       </c>
       <c r="F63" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>478</v>
+        <v>535</v>
       </c>
       <c r="D64" t="s">
         <v>333</v>
       </c>
       <c r="E64" t="s">
-        <v>548</v>
+        <v>519</v>
       </c>
       <c r="F64" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
-        <v>479</v>
+        <v>537</v>
       </c>
       <c r="D65" t="s">
         <v>333</v>
       </c>
       <c r="E65" t="s">
-        <v>548</v>
+        <v>519</v>
       </c>
       <c r="F65" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="C67" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D67" t="s">
         <v>333</v>
       </c>
       <c r="E67" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F67" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="C68" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D68" t="s">
         <v>333</v>
@@ -20262,15 +20240,15 @@
         <v>30</v>
       </c>
       <c r="F68" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="11" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="C69" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D69" t="s">
         <v>333</v>
@@ -20279,43 +20257,43 @@
         <v>32</v>
       </c>
       <c r="F69" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>392</v>
+        <v>490</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D71" s="13" t="s">
         <v>333</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>488</v>
+        <v>463</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="16" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13" t="s">
         <v>334</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>541</v>
+        <v>512</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>489</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -20328,118 +20306,118 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D74" s="13" t="s">
         <v>333</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>490</v>
+        <v>465</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="16" t="s">
-        <v>491</v>
+        <v>466</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13" t="s">
         <v>356</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>549</v>
+        <v>520</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="52" t="s">
-        <v>538</v>
-      </c>
-      <c r="B77" s="51" t="s">
-        <v>540</v>
+      <c r="A77" s="51" t="s">
+        <v>510</v>
+      </c>
+      <c r="B77" s="50" t="s">
+        <v>525</v>
       </c>
       <c r="C77" t="s">
-        <v>422</v>
-      </c>
-      <c r="D77" s="49" t="s">
+        <v>408</v>
+      </c>
+      <c r="D77" s="48" t="s">
         <v>333</v>
       </c>
       <c r="E77" t="s">
-        <v>528</v>
-      </c>
-      <c r="F77" s="50" t="s">
-        <v>539</v>
+        <v>501</v>
+      </c>
+      <c r="F77" s="49" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="53" t="s">
-        <v>388</v>
+      <c r="B78" s="54" t="s">
+        <v>532</v>
       </c>
       <c r="C78" t="s">
-        <v>423</v>
-      </c>
-      <c r="D78" s="49" t="s">
+        <v>409</v>
+      </c>
+      <c r="D78" s="48" t="s">
         <v>333</v>
       </c>
       <c r="E78" t="s">
-        <v>528</v>
-      </c>
-      <c r="F78" s="50" t="s">
-        <v>444</v>
+        <v>501</v>
+      </c>
+      <c r="F78" s="49" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="D79" s="49" t="s">
+        <v>507</v>
+      </c>
+      <c r="D79" s="48" t="s">
         <v>334</v>
       </c>
       <c r="E79" t="s">
-        <v>550</v>
+        <v>521</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>537</v>
+        <v>509</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="D80" s="49" t="s">
+      <c r="D80" s="48" t="s">
         <v>334</v>
       </c>
       <c r="E80" t="s">
-        <v>550</v>
+        <v>521</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="43"/>
-      <c r="D81" s="49"/>
+      <c r="D81" s="48"/>
       <c r="F81" s="12"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="43"/>
-      <c r="D82" s="49"/>
+      <c r="D82" s="48"/>
       <c r="F82" s="12"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="43"/>
-      <c r="D83" s="49"/>
+      <c r="D83" s="48"/>
       <c r="F83" s="12"/>
     </row>
   </sheetData>
@@ -20452,8 +20430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="G161" sqref="G161"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C143" sqref="C142:C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20469,7 +20447,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -20481,13 +20459,13 @@
         <v>359</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>340</v>
@@ -20575,7 +20553,7 @@
         <v>336</v>
       </c>
       <c r="G6" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -20596,7 +20574,7 @@
         <v>336</v>
       </c>
       <c r="H7" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -20617,7 +20595,7 @@
         <v>336</v>
       </c>
       <c r="G8" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -20638,7 +20616,7 @@
         <v>371</v>
       </c>
       <c r="G9" t="s">
-        <v>525</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -20659,7 +20637,7 @@
         <v>341</v>
       </c>
       <c r="G10" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -20680,7 +20658,7 @@
         <v>341</v>
       </c>
       <c r="G11" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -20755,7 +20733,7 @@
         <v>341</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -20776,7 +20754,7 @@
         <v>336</v>
       </c>
       <c r="H16" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -20818,7 +20796,7 @@
         <v>337</v>
       </c>
       <c r="H18" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -20858,51 +20836,51 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46">
+      <c r="A21" s="45">
         <v>18</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="E21" s="45" t="s">
-        <v>467</v>
-      </c>
-      <c r="F21" s="45" t="s">
-        <v>396</v>
-      </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="48" t="s">
-        <v>468</v>
+      <c r="E21" s="44" t="s">
+        <v>453</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>382</v>
+      </c>
+      <c r="G21" s="44"/>
+      <c r="H21" s="47" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="46">
+      <c r="A22" s="45">
         <v>19</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="E22" s="45" t="s">
-        <v>467</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>396</v>
-      </c>
-      <c r="G22" s="48"/>
-      <c r="H22" s="45" t="s">
-        <v>469</v>
+      <c r="E22" s="44" t="s">
+        <v>453</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>382</v>
+      </c>
+      <c r="G22" s="47"/>
+      <c r="H22" s="44" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -20923,10 +20901,10 @@
         <v>336</v>
       </c>
       <c r="F23" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="G23" t="s">
-        <v>526</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -20947,7 +20925,7 @@
         <v>337</v>
       </c>
       <c r="G24" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -20968,7 +20946,7 @@
         <v>337</v>
       </c>
       <c r="G25" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -20989,7 +20967,7 @@
         <v>337</v>
       </c>
       <c r="G26" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -21036,16 +21014,16 @@
         <v>350</v>
       </c>
       <c r="E30" t="s">
-        <v>534</v>
+        <v>506</v>
       </c>
       <c r="F30" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="G30" t="s">
         <v>354</v>
       </c>
       <c r="H30" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -21060,7 +21038,7 @@
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -21075,7 +21053,7 @@
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -21102,7 +21080,7 @@
         <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -21168,7 +21146,7 @@
         <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -21183,7 +21161,7 @@
         <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -21210,7 +21188,7 @@
         <v>67</v>
       </c>
       <c r="F42" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -21336,10 +21314,10 @@
         <v>339</v>
       </c>
       <c r="E52" t="s">
-        <v>553</v>
+        <v>524</v>
       </c>
       <c r="F52" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="H52" t="s">
         <v>353</v>
@@ -21372,10 +21350,10 @@
         <v>339</v>
       </c>
       <c r="E54" t="s">
-        <v>553</v>
+        <v>524</v>
       </c>
       <c r="F54" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="H54" t="s">
         <v>355</v>
@@ -21386,13 +21364,13 @@
         <v>357</v>
       </c>
       <c r="D56" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="E56" t="s">
-        <v>551</v>
+        <v>522</v>
       </c>
       <c r="F56" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="G56" t="s">
         <v>363</v>
@@ -21694,10 +21672,10 @@
         <v>360</v>
       </c>
       <c r="E82" t="s">
-        <v>552</v>
+        <v>523</v>
       </c>
       <c r="F82" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="G82" t="s">
         <v>363</v>
@@ -21853,7 +21831,7 @@
         <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>504</v>
+        <v>479</v>
       </c>
       <c r="C95" t="s">
         <v>165</v>
@@ -21871,7 +21849,7 @@
         <v>167</v>
       </c>
       <c r="G96" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -21946,7 +21924,7 @@
         <v>178</v>
       </c>
       <c r="G102" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -22153,10 +22131,10 @@
         <v>211</v>
       </c>
       <c r="F119" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="H119" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -22171,7 +22149,7 @@
         <v>213</v>
       </c>
       <c r="F120" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -22186,7 +22164,7 @@
         <v>215</v>
       </c>
       <c r="F121" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -22201,7 +22179,7 @@
         <v>217</v>
       </c>
       <c r="F122" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -22216,7 +22194,7 @@
         <v>219</v>
       </c>
       <c r="F123" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -22231,7 +22209,7 @@
         <v>221</v>
       </c>
       <c r="F124" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -22246,7 +22224,7 @@
         <v>223</v>
       </c>
       <c r="F125" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -22261,7 +22239,7 @@
         <v>225</v>
       </c>
       <c r="F126" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -22276,7 +22254,7 @@
         <v>227</v>
       </c>
       <c r="F127" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -22294,10 +22272,10 @@
         <v>334</v>
       </c>
       <c r="F128" s="12" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="G128" t="s">
-        <v>499</v>
+        <v>474</v>
       </c>
       <c r="H128" s="12" t="s">
         <v>361</v>
@@ -22350,10 +22328,10 @@
         <v>360</v>
       </c>
       <c r="E133" t="s">
-        <v>502</v>
+        <v>477</v>
       </c>
       <c r="F133" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="G133" t="s">
         <v>363</v>
@@ -22554,7 +22532,7 @@
         <v>356</v>
       </c>
       <c r="E149" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -22608,7 +22586,7 @@
         <v>356</v>
       </c>
       <c r="E153" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -22662,7 +22640,7 @@
         <v>356</v>
       </c>
       <c r="E157" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -22716,7 +22694,7 @@
         <v>356</v>
       </c>
       <c r="E161" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -22839,7 +22817,7 @@
         <v>311</v>
       </c>
       <c r="F171" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -22854,7 +22832,7 @@
         <v>313</v>
       </c>
       <c r="F172" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -22869,7 +22847,7 @@
         <v>315</v>
       </c>
       <c r="F173" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -22895,13 +22873,13 @@
         <v>336</v>
       </c>
       <c r="F176" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="G176" t="s">
         <v>365</v>
       </c>
       <c r="H176" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="177" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -22919,10 +22897,10 @@
         <v>334</v>
       </c>
       <c r="E177" s="12" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="F177" s="12" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="178" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -22940,10 +22918,10 @@
         <v>334</v>
       </c>
       <c r="E178" s="12" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="F178" s="12" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="179" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -22961,10 +22939,10 @@
         <v>334</v>
       </c>
       <c r="E179" s="12" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="F179" s="12" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="180" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -22982,10 +22960,10 @@
         <v>334</v>
       </c>
       <c r="E180" s="12" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="F180" s="12" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="H180" s="12" t="s">
         <v>366</v>
@@ -23006,10 +22984,10 @@
         <v>334</v>
       </c>
       <c r="E181" s="12" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="F181" s="12" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="H181" s="12" t="s">
         <v>366</v>
@@ -23030,10 +23008,10 @@
         <v>334</v>
       </c>
       <c r="E182" s="12" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="F182" s="12" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="H182" s="12" t="s">
         <v>367</v>

</xml_diff>